<commit_message>
Update LSA Data Dictionary FY2019.xlsx
Closes #294
closes #299
closes #290
closes #438
closes #432
closes #434
</commit_message>
<xml_diff>
--- a/LSA Data Dictionary FY2019.xlsx
+++ b/LSA Data Dictionary FY2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/84a436417b82d0fe/GitHub/LSASampleCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFCBF1A5-9043-4C5C-B1DD-C2D2BC6E3DF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{DFCBF1A5-9043-4C5C-B1DD-C2D2BC6E3DF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{54C71EB9-2B22-4E8D-852D-61E5891E9EC3}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6465" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -3713,7 +3713,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D516"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118:XFD118"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -10960,8 +10962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="D208" sqref="D208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17208,21 +17210,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7BB265D7978C04697446D294C34266E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="884d559af15d355cca1525f15b65ea2d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="77672a2e-0500-447c-bfb5-fe50f00aefa9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8903f88819ac4802e9a17e43e02e9a2c" ns2:_="">
     <xsd:import namespace="77672a2e-0500-447c-bfb5-fe50f00aefa9"/>
@@ -17368,24 +17355,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4CF5C08-B8BD-4ACA-92AF-480DA74E9990}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{378C2C19-6654-4992-87BB-EE419392A4EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C6275C-4ECA-4DA0-9DFB-79D242E0383C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17401,4 +17386,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{378C2C19-6654-4992-87BB-EE419392A4EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4CF5C08-B8BD-4ACA-92AF-480DA74E9990}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>